<commit_message>
add side channel data
</commit_message>
<xml_diff>
--- a/experiment_data/SECRET-GWAS Data.xlsx
+++ b/experiment_data/SECRET-GWAS Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JRose/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JRose/Desktop/SECRET-GWAS/experiment_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9CECE89-DFBA-BF49-A668-BD72788F4F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFC7E95-7653-6747-AF49-74E909EBC130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="8" xr2:uid="{7EA522C4-4F4C-F24F-83B1-BFF66797546D}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" firstSheet="4" activeTab="8" xr2:uid="{7EA522C4-4F4C-F24F-83B1-BFF66797546D}"/>
   </bookViews>
   <sheets>
     <sheet name="Network Breakdown" sheetId="1" state="hidden" r:id="rId1"/>
@@ -21,9 +21,10 @@
     <sheet name="Log Reg Overhead" sheetId="14" r:id="rId6"/>
     <sheet name="Lin Reg Overhead" sheetId="10" r:id="rId7"/>
     <sheet name="Combined Overhead Fig." sheetId="19" r:id="rId8"/>
-    <sheet name="SECRET-GWAS CSV" sheetId="4" r:id="rId9"/>
-    <sheet name="Not GLORE (wink) " sheetId="5" state="hidden" r:id="rId10"/>
-    <sheet name="New SGX Overhead" sheetId="6" state="hidden" r:id="rId11"/>
+    <sheet name="EPC" sheetId="4" r:id="rId9"/>
+    <sheet name="Side Channel" sheetId="20" r:id="rId10"/>
+    <sheet name="Not GLORE (wink) " sheetId="5" state="hidden" r:id="rId11"/>
+    <sheet name="New SGX Overhead" sheetId="6" state="hidden" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="96">
   <si>
     <t>Log</t>
   </si>
@@ -301,6 +302,39 @@
   </si>
   <si>
     <t>no-sgx-spec-mit-20k</t>
+  </si>
+  <si>
+    <t>Oblivious</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>DET</t>
   </si>
 </sst>
 </file>
@@ -17290,7 +17324,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -17359,7 +17393,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$B$2:$B$21</c:f>
+              <c:f>EPC!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -17451,7 +17485,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -17520,7 +17554,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$C$2:$C$21</c:f>
+              <c:f>EPC!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -17626,7 +17660,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -17695,7 +17729,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$D$2:$D$21</c:f>
+              <c:f>EPC!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -17778,7 +17812,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -17847,7 +17881,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$E$2:$E$21</c:f>
+              <c:f>EPC!$E$2:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -17953,7 +17987,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18022,7 +18056,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$F$2:$F$21</c:f>
+              <c:f>EPC!$F$2:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18090,7 +18124,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18159,7 +18193,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$G$2:$G$21</c:f>
+              <c:f>EPC!$G$2:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18254,7 +18288,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18323,7 +18357,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$H$2:$H$21</c:f>
+              <c:f>EPC!$H$2:$H$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18388,7 +18422,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18457,7 +18491,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$I$2:$I$21</c:f>
+              <c:f>EPC!$I$2:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18540,7 +18574,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18609,7 +18643,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$J$2:$J$21</c:f>
+              <c:f>EPC!$J$2:$J$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18668,7 +18702,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18737,7 +18771,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$K$2:$K$21</c:f>
+              <c:f>EPC!$K$2:$K$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18816,7 +18850,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18885,7 +18919,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$L$2:$L$21</c:f>
+              <c:f>EPC!$L$2:$L$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -18941,7 +18975,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -19010,7 +19044,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$M$2:$M$21</c:f>
+              <c:f>EPC!$M$2:$M$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -19083,7 +19117,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$A$2:$A$21</c:f>
+              <c:f>EPC!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -19152,7 +19186,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SECRET-GWAS CSV'!$N$2:$N$21</c:f>
+              <c:f>EPC!$N$2:$N$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -53671,6 +53705,269 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D774DF9D-F689-7041-9119-1593653702A1}">
+  <dimension ref="A2:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5825.4356440000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>58.28</v>
+      </c>
+      <c r="D4" s="1">
+        <v>11.18295694</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.5241686489999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5830.33</v>
+      </c>
+      <c r="C5" s="1">
+        <v>202.03</v>
+      </c>
+      <c r="D5" s="1">
+        <v>18.27347426</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6.631916199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5827.75</v>
+      </c>
+      <c r="C6" s="1">
+        <v>369.6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>17.92026736</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16.973136499999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5839.05</v>
+      </c>
+      <c r="C7" s="1">
+        <v>446.38</v>
+      </c>
+      <c r="D7" s="1">
+        <v>24.111295699999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4.8540979450000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5837.26</v>
+      </c>
+      <c r="C8" s="1">
+        <v>572.95049500000005</v>
+      </c>
+      <c r="D8" s="1">
+        <v>21.283116979999999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>11.25222379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5833.7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>683.01980200000003</v>
+      </c>
+      <c r="D9" s="1">
+        <v>16.19184297</v>
+      </c>
+      <c r="E9" s="1">
+        <v>12.078239480000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9142.8415839999998</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4606.99</v>
+      </c>
+      <c r="D12" s="1">
+        <v>24.628491650000001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>20.909788729999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="1">
+        <v>9151.6138609999998</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4875.53</v>
+      </c>
+      <c r="D13" s="1">
+        <v>23.661866960000001</v>
+      </c>
+      <c r="E13" s="1">
+        <v>18.643980989999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9151.43</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4749.34</v>
+      </c>
+      <c r="D14" s="1">
+        <v>16.88746905</v>
+      </c>
+      <c r="E14" s="1">
+        <v>7.2201088100000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="1">
+        <v>9150.636364</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4705.47</v>
+      </c>
+      <c r="D15" s="1">
+        <v>27.282629180000001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>15.529883679999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="1">
+        <v>9140.19</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4629.04</v>
+      </c>
+      <c r="D16" s="1">
+        <v>36.5557923</v>
+      </c>
+      <c r="E16" s="1">
+        <v>8.4001995619999992</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="1">
+        <v>9153.84</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4395.8100000000004</v>
+      </c>
+      <c r="D17" s="1">
+        <v>26.242291170000001</v>
+      </c>
+      <c r="E17" s="1">
+        <v>7.3839361060000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93404B4D-170F-E04A-9EF3-B8471A0A3F68}">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -53735,7 +54032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6EBB29-0B1C-4143-8770-1C97A2547218}">
   <dimension ref="A1:O37"/>
   <sheetViews>

</xml_diff>